<commit_message>
Citynames, area names, various improvements, added testing. Nearing the end :-)
</commit_message>
<xml_diff>
--- a/excel/Geopackages.xlsx
+++ b/excel/Geopackages.xlsx
@@ -5,14 +5,16 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\htdocs\tileserver\design\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\maps\top10nl\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="11100"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="11100" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="111">
   <si>
     <t>namespace: String (200.0)
 lokaalid: String (160.0)
@@ -1484,12 +1486,46 @@
   typewater (String) = waterloop
   typewater (String) = zee</t>
   </si>
+  <si>
+    <t>Plaatsnamen</t>
+  </si>
+  <si>
+    <t>Schaal</t>
+  </si>
+  <si>
+    <t>punt</t>
+  </si>
+  <si>
+    <t>vlak</t>
+  </si>
+  <si>
+    <t>multivlak</t>
+  </si>
+  <si>
+    <t>Totaal</t>
+  </si>
+  <si>
+    <t>&gt;25000</t>
+  </si>
+  <si>
+    <t>&gt;5000</t>
+  </si>
+  <si>
+    <t>&lt;10000</t>
+  </si>
+  <si>
+    <t>Plaat tekstgrootte</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.0_-;\-* #,##0.0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1499,6 +1535,13 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -1529,18 +1572,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1821,8 +1867,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B26" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="D26" sqref="D26"/>
@@ -2242,4 +2288,222 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>102</v>
+      </c>
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" t="s">
+        <v>103</v>
+      </c>
+      <c r="D4" t="s">
+        <v>104</v>
+      </c>
+      <c r="E4" t="s">
+        <v>105</v>
+      </c>
+      <c r="F4" t="s">
+        <v>106</v>
+      </c>
+      <c r="H4" t="s">
+        <v>103</v>
+      </c>
+      <c r="I4" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>10</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>2589</v>
+      </c>
+      <c r="E5">
+        <v>158</v>
+      </c>
+      <c r="F5">
+        <f>SUM(C5:E5)</f>
+        <v>2747</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>250</v>
+      </c>
+      <c r="C6">
+        <v>1949</v>
+      </c>
+      <c r="D6">
+        <v>659</v>
+      </c>
+      <c r="F6">
+        <f t="shared" ref="F6:F8" si="0">SUM(C6:E6)</f>
+        <v>2608</v>
+      </c>
+      <c r="H6" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>500</v>
+      </c>
+      <c r="C7">
+        <v>699</v>
+      </c>
+      <c r="D7">
+        <v>659</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="0"/>
+        <v>1358</v>
+      </c>
+      <c r="I7" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>1000</v>
+      </c>
+      <c r="C8">
+        <v>1376</v>
+      </c>
+      <c r="D8">
+        <v>121</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="0"/>
+        <v>1497</v>
+      </c>
+      <c r="I8" t="s">
+        <v>107</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:F9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C4">
+        <v>26</v>
+      </c>
+      <c r="E4" s="4">
+        <v>10</v>
+      </c>
+      <c r="F4" s="4">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C5">
+        <v>21</v>
+      </c>
+      <c r="E5" s="4">
+        <f>$C5/$C$4*E$4</f>
+        <v>8.0769230769230766</v>
+      </c>
+      <c r="F5" s="4">
+        <f>$C5/$C$4*F$4</f>
+        <v>80.769230769230774</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C6">
+        <v>18</v>
+      </c>
+      <c r="E6" s="4">
+        <f t="shared" ref="E6:F9" si="0">$C6/$C$4*E$4</f>
+        <v>6.9230769230769234</v>
+      </c>
+      <c r="F6" s="4">
+        <f t="shared" si="0"/>
+        <v>69.230769230769226</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C7">
+        <v>14</v>
+      </c>
+      <c r="E7" s="4">
+        <f t="shared" si="0"/>
+        <v>5.3846153846153841</v>
+      </c>
+      <c r="F7" s="4">
+        <f t="shared" si="0"/>
+        <v>53.846153846153847</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C8">
+        <v>12</v>
+      </c>
+      <c r="E8" s="4">
+        <f t="shared" si="0"/>
+        <v>4.6153846153846159</v>
+      </c>
+      <c r="F8" s="4">
+        <f t="shared" si="0"/>
+        <v>46.153846153846153</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C9">
+        <v>9.5</v>
+      </c>
+      <c r="E9" s="4">
+        <f t="shared" si="0"/>
+        <v>3.6538461538461537</v>
+      </c>
+      <c r="F9" s="4">
+        <f t="shared" si="0"/>
+        <v>36.538461538461533</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>